<commit_message>
Keyword and test case modification according to new orgs url
</commit_message>
<xml_diff>
--- a/TestData/Production/Web_POS/Billing/billing_test_data.xlsx
+++ b/TestData/Production/Web_POS/Billing/billing_test_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="Calc"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\TESTDATA\PRODUCTION\Web_POS\Billing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saloni\Desktop\Ginesys\Zwing_repo\zwing-qa-automation\TestData\Production\Web_POS\Billing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -110,7 +110,7 @@
     <t>239060824oqM</t>
   </si>
   <si>
-    <t>Zwingautomation78@gmail..com</t>
+    <t>Zwingautomation78@gmail.com</t>
   </si>
   <si>
     <t>B_user1_p1</t>
@@ -710,8 +710,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0" topLeftCell="A34">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.542969" defaultRowHeight="12.75"/>

</xml_diff>